<commit_message>
after change new excel file
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>hindi</t>
+  </si>
+  <si>
+    <t>my new change</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +396,7 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -416,7 +419,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -428,7 +431,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -440,7 +443,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -451,6 +454,11 @@
         <v>8</v>
       </c>
       <c r="D5" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>